<commit_message>
update sprint2 RefReq word count
</commit_message>
<xml_diff>
--- a/Documentation/Requirements and Reference/Sprint2_ReqRef.xlsx
+++ b/Documentation/Requirements and Reference/Sprint2_ReqRef.xlsx
@@ -248,7 +248,7 @@
     <t>EECS 581 Project 1 &amp; 2</t>
   </si>
   <si>
-    <t>Setup Github repository. Invite the entire team to be collaborators on the repo. Ensure everyone is able to clone the repo and has write access.</t>
+    <t>Create a GitHub repository, invite all team members as collaborators, and ensure that everyone can successfully clone the repository and has full write access to contribute changes.</t>
   </si>
   <si>
     <t>EECS 168</t>
@@ -266,16 +266,16 @@
     <t>Set up person hours tracker. Come up with required criteria (estimated time vs actual time, description of task, who the task is assigned to) and implement them in a Google spreadsheet</t>
   </si>
   <si>
-    <t xml:space="preserve">Hold weekly scurm meeting to discuss what we completed, any blockers/impediments and next sprint goals. Assign tasks to be completed by the next meeting. </t>
+    <t>Hold weekly scrum meetings to review completed tasks, identify blockers or impediments, set goals for the next sprint, and assign responsibilities to team members for completion before the next meeting.</t>
   </si>
   <si>
-    <t xml:space="preserve">Coordinating weekly meeting times for team and TA meetings. Ensuring everyone is consistently avalible at a common time each week for 1 hour.  </t>
+    <t>Coordinate weekly meeting times for both the team and TA sessions, making sure all members are consistently available for a one-hour meeting each week at a common, agreed-upon time.</t>
   </si>
   <si>
     <t xml:space="preserve">Add buttons to the main menu allowing the player to select whether to play solo, take turns with an AI, or have the AI auto solve. This also includes adding buttons to select which game mode the AI plays on: easy, medium, or hard. </t>
   </si>
   <si>
-    <t xml:space="preserve">Create a high level system architeure document describing the core game components, AI logic layers, and interactions between the game </t>
+    <t>Create a high-level system architecture document detailing the core game components, AI logic layers, and interactions between various game systems to ensure clarity, organization, and efficient team collaboration.</t>
   </si>
   <si>
     <t>Create Easy AI functionality that enables the computer to randomly select and uncover a cell that has not already been revealed or flagged, ensuring basic automated gameplay without using any strategic decision-making or pattern recognition</t>
@@ -299,7 +299,7 @@
     <t>Let the player reveal a cell. Check whether the selected cell contains a mine. If it’s a mine, then game over. If it’s not a mine, then reveal the cell and show the count of nearby mines. If the number is 0, automatically reveal all adjacent non mine cells recursively.</t>
   </si>
   <si>
-    <t>Create UI Mockup of different game state screens using Figma. Mock the game state flow and account for the user winning or losing the game.</t>
+    <t>Design UI mockups in Figma for all game state screens, illustrating the full game flow and transitions, including scenarios where the player either wins or loses the game.</t>
   </si>
   <si>
     <t>After each reveal, update the game board. Maintain separate data structures for the hidden board (true mine locations and numbers) and visible board (what the player currently sees). Track how many safe cells remain unrevealed.</t>

</xml_diff>